<commit_message>
Enhance email automation by adding logging functionality, progress tracking, and improved error handling. Updated GUI to display email sending progress and log messages, while refining recipient data processing from Excel.
</commit_message>
<xml_diff>
--- a/sample_list.xlsx
+++ b/sample_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Email-Automation-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D6D694-21BB-4803-AA4F-F62DB7E71AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428D4B31-8BAF-43C7-A220-DD2FB13647E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1365" windowWidth="27000" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,52 +20,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+  <si>
+    <t>$NAME</t>
+  </si>
   <si>
     <t>Email</t>
   </si>
   <si>
+    <t>$NOTIFICATION_URL</t>
+  </si>
+  <si>
     <t>Đào Duy Thông</t>
   </si>
   <si>
     <t>duythong.ptit@gmail.com</t>
   </si>
   <si>
+    <t>https://so-media-potral.vercel.app/passinterview/-O_75N9xzUIZDYnUcP5j</t>
+  </si>
+  <si>
     <t>Tống Ngọc Kiên</t>
   </si>
   <si>
     <t>duythong020703@gmail.com</t>
   </si>
   <si>
-    <t>https://so-media-potral.vercel.app/passcv/-O_Sl6QoO5_Mtn-Xw_Ja</t>
-  </si>
-  <si>
-    <t>https://so-media-potral.vercel.app/passcv/-O_SjCTkzCnBBkjEs7OW</t>
-  </si>
-  <si>
-    <t>$NAME</t>
-  </si>
-  <si>
-    <t>$NOTIFICATION_URL</t>
+    <t>Vũ Thị Phương Thảo</t>
+  </si>
+  <si>
+    <t>Đào Dương Cẩm Tú</t>
+  </si>
+  <si>
+    <t>Nguyễn Đoan Trang</t>
+  </si>
+  <si>
+    <t>vtphth716@gmail.com</t>
+  </si>
+  <si>
+    <t>kimcotton124@gmail.com</t>
   </si>
   <si>
     <t>ddcamtus216@gmail.com</t>
-  </si>
-  <si>
-    <t>vtphth716@gmail.com</t>
-  </si>
-  <si>
-    <t>Đào Dương Cẩm Tú</t>
-  </si>
-  <si>
-    <t>Vũ Thị Phương Thảo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -96,35 +99,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -132,33 +116,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -378,86 +346,87 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{27F1193B-668C-4914-89E8-38BB2A3327C9}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{C1005ABA-DA90-4F0D-B172-DA27DB05595C}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{13E2075A-775C-496D-9B57-9731AADBD02F}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{3B283CDF-C387-4EE0-8803-940C32104900}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>